<commit_message>
Update with edge routers.
</commit_message>
<xml_diff>
--- a/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
+++ b/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynns/sources/git/canu/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynns/sources/git/canu/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A46930BF-F13E-0842-9D82-5ADC8E1B94BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF73A91-11BD-144E-9FF7-4673475F1CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
   </bookViews>
   <sheets>
     <sheet name="INTER_SWITCH_LINKS" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="51">
   <si>
     <t>Source</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>u37</t>
+  </si>
+  <si>
+    <t>x3003</t>
+  </si>
+  <si>
+    <t>sw-edge-001</t>
+  </si>
+  <si>
+    <t>sw-edge-002</t>
   </si>
 </sst>
 </file>
@@ -564,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807AEA7A-78A2-1142-B8D3-13084383B4B0}">
-  <dimension ref="J14:U38"/>
+  <dimension ref="J14:U42"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1302,6 +1311,110 @@
       </c>
       <c r="T38" s="2">
         <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O39" s="2">
+        <v>1</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T39" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J40" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O40" s="2">
+        <v>1</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T40" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O41" s="2">
+        <v>2</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T41" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O42" s="2">
+        <v>2</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T42" s="2">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2777,7 +2890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE6AFE8-EB28-2149-9C5F-BA9B2992165A}">
   <dimension ref="J14:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add leaf-bmc to leaf connections and fix cmm ports
</commit_message>
<xml_diff>
--- a/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
+++ b/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynns/sources/git/canu/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF73A91-11BD-144E-9FF7-4673475F1CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626AA3D2-5F38-5E43-9124-136C8CF01EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
   </bookViews>
   <sheets>
     <sheet name="INTER_SWITCH_LINKS" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="51">
   <si>
     <t>Source</t>
   </si>
@@ -573,15 +573,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807AEA7A-78A2-1142-B8D3-13084383B4B0}">
-  <dimension ref="J14:U42"/>
+  <dimension ref="J14:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1415,6 +1415,58 @@
       </c>
       <c r="T42" s="2">
         <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O43" s="2">
+        <v>48</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T43" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="10:21" x14ac:dyDescent="0.2">
+      <c r="J44" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O44" s="2">
+        <v>47</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T44" s="2">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1426,7 +1478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C3018C-CE0C-E04E-8947-8C874399EC7B}">
   <dimension ref="J14:T48"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" workbookViewId="0">
+    <sheetView topLeftCell="B14" workbookViewId="0">
       <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
@@ -2532,8 +2584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7990636-0CF9-6941-8EF6-80CF48D8BDA7}">
   <dimension ref="J14:T24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16:R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2596,7 +2648,7 @@
         <v>18</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="2">
@@ -2627,7 +2679,7 @@
         <v>18</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="2">
@@ -2658,7 +2710,7 @@
         <v>18</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="S17" s="2"/>
       <c r="T17" s="2">
@@ -2689,7 +2741,7 @@
         <v>18</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="2">
@@ -2720,7 +2772,7 @@
         <v>18</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="S19" s="2"/>
       <c r="T19" s="2">
@@ -2751,7 +2803,7 @@
         <v>18</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="2">
@@ -2782,7 +2834,7 @@
         <v>18</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="S21" s="2"/>
       <c r="T21" s="2">
@@ -2813,7 +2865,7 @@
         <v>18</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="S22" s="2"/>
       <c r="T22" s="2">
@@ -2844,7 +2896,7 @@
         <v>18</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="S23" s="2"/>
       <c r="T23" s="2">
@@ -2874,7 +2926,7 @@
         <v>18</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="2">
@@ -2890,8 +2942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE6AFE8-EB28-2149-9C5F-BA9B2992165A}">
   <dimension ref="J14:U23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3077,7 +3129,7 @@
         <v>47</v>
       </c>
       <c r="O20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P20" s="2" t="s">
         <v>40</v>
@@ -3103,7 +3155,7 @@
         <v>24</v>
       </c>
       <c r="O21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>40</v>
@@ -3129,7 +3181,7 @@
         <v>25</v>
       </c>
       <c r="O22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>40</v>
@@ -3155,7 +3207,7 @@
         <v>26</v>
       </c>
       <c r="O23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P23" s="2" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Correct ocp and pcie-slot1 port 2 connections for masters.
</commit_message>
<xml_diff>
--- a/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
+++ b/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynns/sources/git/canu/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626AA3D2-5F38-5E43-9124-136C8CF01EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207B74BC-5555-C742-9237-7BA9B845F838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
   </bookViews>
   <sheets>
     <sheet name="INTER_SWITCH_LINKS" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="52">
   <si>
     <t>Source</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>sw-edge-002</t>
+  </si>
+  <si>
+    <t>SITE</t>
   </si>
 </sst>
 </file>
@@ -1478,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C3018C-CE0C-E04E-8947-8C874399EC7B}">
   <dimension ref="J14:T48"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1570,7 +1573,7 @@
         <v>2</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>18</v>
@@ -1580,7 +1583,7 @@
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="10:20" x14ac:dyDescent="0.2">
@@ -1632,7 +1635,7 @@
         <v>2</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="Q18" s="2" t="s">
         <v>18</v>
@@ -1642,7 +1645,7 @@
       </c>
       <c r="S18" s="2"/>
       <c r="T18" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="10:20" x14ac:dyDescent="0.2">
@@ -1694,7 +1697,7 @@
         <v>2</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>18</v>
@@ -1704,7 +1707,7 @@
       </c>
       <c r="S20" s="2"/>
       <c r="T20" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="10:20" x14ac:dyDescent="0.2">
@@ -1756,7 +1759,7 @@
         <v>2</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="Q22" s="2" t="s">
         <v>18</v>
@@ -1766,7 +1769,7 @@
       </c>
       <c r="S22" s="2"/>
       <c r="T22" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="10:20" x14ac:dyDescent="0.2">
@@ -1818,7 +1821,7 @@
         <v>2</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="Q24" s="2" t="s">
         <v>19</v>
@@ -1828,7 +1831,7 @@
       </c>
       <c r="S24" s="2"/>
       <c r="T24" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="10:20" x14ac:dyDescent="0.2">
@@ -1880,7 +1883,7 @@
         <v>2</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>19</v>
@@ -1890,7 +1893,7 @@
       </c>
       <c r="S26" s="2"/>
       <c r="T26" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="10:20" x14ac:dyDescent="0.2">
@@ -2942,7 +2945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE6AFE8-EB28-2149-9C5F-BA9B2992165A}">
   <dimension ref="J14:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add BMC ports to river compute and add tests.
</commit_message>
<xml_diff>
--- a/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
+++ b/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynns/sources/git/canu/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynns/sources/git/canu/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207B74BC-5555-C742-9237-7BA9B845F838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ABC195-7A7B-254B-B344-4A7A4EFE653B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
   </bookViews>
   <sheets>
     <sheet name="INTER_SWITCH_LINKS" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="60">
   <si>
     <t>Source</t>
   </si>
@@ -193,6 +193,30 @@
   </si>
   <si>
     <t>SITE</t>
+  </si>
+  <si>
+    <t>cn01</t>
+  </si>
+  <si>
+    <t>cn02</t>
+  </si>
+  <si>
+    <t>cn03</t>
+  </si>
+  <si>
+    <t>cn04</t>
+  </si>
+  <si>
+    <t>u15</t>
+  </si>
+  <si>
+    <t>u16</t>
+  </si>
+  <si>
+    <t>u17</t>
+  </si>
+  <si>
+    <t>u18</t>
   </si>
 </sst>
 </file>
@@ -1481,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C3018C-CE0C-E04E-8947-8C874399EC7B}">
   <dimension ref="J14:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+    <sheetView topLeftCell="J15" workbookViewId="0">
       <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
@@ -2585,10 +2609,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7990636-0CF9-6941-8EF6-80CF48D8BDA7}">
-  <dimension ref="J14:T24"/>
+  <dimension ref="J14:T28"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16:R24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2936,6 +2960,126 @@
         <v>10</v>
       </c>
     </row>
+    <row r="25" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" s="2">
+        <v>1</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" s="2">
+        <v>1</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O27" s="2">
+        <v>1</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O28" s="2">
+        <v>1</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2943,10 +3087,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE6AFE8-EB28-2149-9C5F-BA9B2992165A}">
-  <dimension ref="J14:U23"/>
+  <dimension ref="J14:U27"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="M24" sqref="M24:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3225,6 +3369,118 @@
         <v>5</v>
       </c>
     </row>
+    <row r="24" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="O24" s="2">
+        <v>1</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="O25" s="2">
+        <v>1</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="O26" s="2">
+        <v>1</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="O27" s="2">
+        <v>1</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add BMC ports to river compute and add tests. (#17)
</commit_message>
<xml_diff>
--- a/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
+++ b/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynns/sources/git/canu/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynns/sources/git/canu/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207B74BC-5555-C742-9237-7BA9B845F838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ABC195-7A7B-254B-B344-4A7A4EFE653B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
   </bookViews>
   <sheets>
     <sheet name="INTER_SWITCH_LINKS" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="60">
   <si>
     <t>Source</t>
   </si>
@@ -193,6 +193,30 @@
   </si>
   <si>
     <t>SITE</t>
+  </si>
+  <si>
+    <t>cn01</t>
+  </si>
+  <si>
+    <t>cn02</t>
+  </si>
+  <si>
+    <t>cn03</t>
+  </si>
+  <si>
+    <t>cn04</t>
+  </si>
+  <si>
+    <t>u15</t>
+  </si>
+  <si>
+    <t>u16</t>
+  </si>
+  <si>
+    <t>u17</t>
+  </si>
+  <si>
+    <t>u18</t>
   </si>
 </sst>
 </file>
@@ -1481,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C3018C-CE0C-E04E-8947-8C874399EC7B}">
   <dimension ref="J14:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+    <sheetView topLeftCell="J15" workbookViewId="0">
       <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
@@ -2585,10 +2609,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7990636-0CF9-6941-8EF6-80CF48D8BDA7}">
-  <dimension ref="J14:T24"/>
+  <dimension ref="J14:T28"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16:R24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2936,6 +2960,126 @@
         <v>10</v>
       </c>
     </row>
+    <row r="25" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" s="2">
+        <v>1</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O26" s="2">
+        <v>1</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O27" s="2">
+        <v>1</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O28" s="2">
+        <v>1</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2943,10 +3087,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE6AFE8-EB28-2149-9C5F-BA9B2992165A}">
-  <dimension ref="J14:U23"/>
+  <dimension ref="J14:U27"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="M24" sqref="M24:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3225,6 +3369,118 @@
         <v>5</v>
       </c>
     </row>
+    <row r="24" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="O24" s="2">
+        <v>1</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="O25" s="2">
+        <v>1</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="O26" s="2">
+        <v>1</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="10:20" x14ac:dyDescent="0.2">
+      <c r="J27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="O27" s="2">
+        <v>1</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added dellanox MTN templates
</commit_message>
<xml_diff>
--- a/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
+++ b/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynns/sources/git/canu/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasbates/canu-container/canu/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ABC195-7A7B-254B-B344-4A7A4EFE653B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B85433-88C2-5541-896A-25DCAE9B1E2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="28040" windowHeight="17040" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
   </bookViews>
   <sheets>
-    <sheet name="INTER_SWITCH_LINKS" sheetId="4" r:id="rId1"/>
+    <sheet name="SWITCH_TO_SWITCH" sheetId="4" r:id="rId1"/>
     <sheet name="NON_COMPUTE_NODES" sheetId="1" r:id="rId2"/>
     <sheet name="HARDWARE_MANAGEMENT" sheetId="3" r:id="rId3"/>
     <sheet name="COMPUTE_NODES" sheetId="2" r:id="rId4"/>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807AEA7A-78A2-1142-B8D3-13084383B4B0}">
   <dimension ref="J14:U44"/>
   <sheetViews>
-    <sheetView topLeftCell="C12" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2611,7 +2611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7990636-0CF9-6941-8EF6-80CF48D8BDA7}">
   <dimension ref="J14:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CASMNET-858: Create initial Dell and Mellanox configuration templates - WIP (#12)
* dell-mellanox phase 1

* dellanox phase 2

* moving files

* remove old files

* phase to relocate files, new variables

* fixes as per Lukes review

* fix build error

* fixes roud 2

* dell mellanox config gen first pass

* update requirements

* update test requirements

* rpm build update

* lint

* update docs for Dell and Mellanox

* added extra configs

* fixed sw-leaf-bmc config template

* dellanox template updates

* added dellanox MTN templates

* Added dellanox MTN templates

Co-authored-by: kosonenj <jouni.kosonen@hpe.com>
Co-authored-by: Brooks Vinyard <8202653+brooksvinyard@users.noreply.github.com>
Co-authored-by: lukebates123 <lucas.bates@hpe.com>
</commit_message>
<xml_diff>
--- a/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
+++ b/tests/data/Full_Architecture_Golden_Config_0.0.6.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynns/sources/git/canu/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasbates/canu-container/canu/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ABC195-7A7B-254B-B344-4A7A4EFE653B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B85433-88C2-5541-896A-25DCAE9B1E2E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="28040" windowHeight="17040" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
   </bookViews>
   <sheets>
-    <sheet name="INTER_SWITCH_LINKS" sheetId="4" r:id="rId1"/>
+    <sheet name="SWITCH_TO_SWITCH" sheetId="4" r:id="rId1"/>
     <sheet name="NON_COMPUTE_NODES" sheetId="1" r:id="rId2"/>
     <sheet name="HARDWARE_MANAGEMENT" sheetId="3" r:id="rId3"/>
     <sheet name="COMPUTE_NODES" sheetId="2" r:id="rId4"/>
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807AEA7A-78A2-1142-B8D3-13084383B4B0}">
   <dimension ref="J14:U44"/>
   <sheetViews>
-    <sheetView topLeftCell="C12" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2611,7 +2611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7990636-0CF9-6941-8EF6-80CF48D8BDA7}">
   <dimension ref="J14:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>

</xml_diff>